<commit_message>
add uniprot to supp tables
</commit_message>
<xml_diff>
--- a/supplementary-material/supplementary-table1.xlsx
+++ b/supplementary-material/supplementary-table1.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaaminivenkataraman/Documents/project-EWD-transcriptomics/supplemental-material/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaaminivenkataraman/Documents/project-EWD-transcriptomics/supplementary-material/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6000E108-8A54-EA41-BA30-75F380EC13FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CB839C-B0F8-3E47-A58D-C2BFC6812F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="DE.EXP.CON.FDR.Z.Annot.M" sheetId="1" r:id="rId1"/>
+    <sheet name="differentially-expressed-genes" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
@@ -11320,7 +11320,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -12155,10 +12155,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P541"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -38584,5 +38586,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>